<commit_message>
Revert "R0200 Oxaloacetate decarboxylase"
This reverts commit 512f8ed5bcf00af14d1e594034c3557f984836ec.
</commit_message>
<xml_diff>
--- a/iFermentAsPacidpropionici.xlsx
+++ b/iFermentAsPacidpropionici.xlsx
@@ -1218,7 +1218,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.2644993817742729</v>
+        <v>-1.749529265654429</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.1561110347869477</v>
+        <v>0.8615440086535034</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.1409265432143405</v>
+        <v>-0.8699571331276832</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.1409265432143406</v>
+        <v>-0.8699571331276833</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.1235728385599323</v>
+        <v>-0.8795721325267457</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-1</v>
+        <v>-1.000000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.5681096754134138</v>
+        <v>3.604823524698546</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.8326090571876869</v>
+        <v>1.855294259044117</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.8326090571876869</v>
+        <v>1.855294259044117</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.8326090571876869</v>
+        <v>1.855294259044118</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1.720243819550394</v>
+        <v>2.793037137935192</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>-1.720243819550394</v>
+        <v>-2.793037137935192</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-1.663410436807207</v>
+        <v>-2.761548014903262</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>1.663410436807206</v>
+        <v>2.761548014903262</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.5627589498116394</v>
+        <v>1.705781018388694</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-0.0607379662904288</v>
+        <v>-0.03365249789671901</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.01258143587444597</v>
+        <v>0.006970874564320367</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.01865523250348885</v>
+        <v>0.4106806618324632</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.4003445374784709</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.2342171671523991</v>
+        <v>1.534313529105413</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-6.477584094111134e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0.2408549591826183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>1.010592990549451</v>
+        <v>-0.008893874444132883</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>1.026645167354779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>0.2408549591826183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>0.2408549591826182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>0.2408549591826182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>-2.844116822242711</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-1.678609389800341</v>
+        <v>-0.7966027002123338</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>1.678609389800341</v>
+        <v>0.7966027002123338</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>2.496865487096881</v>
+        <v>4.192500300468752</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0.1014613265461113</v>
+        <v>1.060414246224113</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0.1014613265461113</v>
+        <v>1.060414246224113</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>-1.010592990549451</v>
+        <v>0.008893874444132883</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>2.364286060619462e-15</v>
+        <v>2.881211122307894e-16</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>5.688233644485422</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-0.3739723353024972</v>
+        <v>-0.2072032370497985</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>0.3739723353024972</v>
+        <v>0.2072032370497985</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.009110694943564321</v>
+        <v>-0.005047874684507852</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0.009110694943564319</v>
+        <v>0.005047874684507852</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0.2056414001547375</v>
+        <v>0.1139377428788915</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-0.03731046500697907</v>
+        <v>-0.02067224870798434</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0.03731046500697907</v>
+        <v>0.02067224870798434</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0.04338426163602057</v>
+        <v>0.02403749849765644</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0.04338426163602057</v>
+        <v>0.02403749849765644</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0.01258143587444597</v>
+        <v>0.006970874564320367</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>0.01865523250348885</v>
+        <v>0.4106806618324632</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2346,7 +2346,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>0.2408549591826183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2466,7 +2466,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>0.836491948604128</v>
+        <v>1.032290372981856</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2490,7 +2490,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>0.836491948604128</v>
+        <v>1.032290372981856</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>1.388281910932199</v>
+        <v>2.742558391090113</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>1.56183341889674</v>
+        <v>3.709466768158342</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>-1.561833418896741</v>
+        <v>-0.8653499459156319</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>-0.05070174043196746</v>
+        <v>-1.032290372981856</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2690,7 +2690,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>0.1678103240081669</v>
+        <v>1.799447137534562</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>-0.9605709368831467</v>
+        <v>-1.101037618685153</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>-0.1171085835761996</v>
+        <v>-0.7671567645527064</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2778,7 +2778,7 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>0.2408549591826183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0.9999999999999998</v>
+        <v>1.000000000000005</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2826,7 +2826,7 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>-0.2408549591826183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>0.4206104165612206</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>0.4206104165612206</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2930,7 +2930,7 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>0.4206104165612206</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>0.4206104165612206</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="230" spans="1:2">

</xml_diff>

<commit_message>
Removing remaining knock outs from iFerment
Missed three additional reactions that should have been commented in iFerment, since knock outs are handled in assignments code
</commit_message>
<xml_diff>
--- a/iFermentAsPacidpropionici.xlsx
+++ b/iFermentAsPacidpropionici.xlsx
@@ -1218,7 +1218,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-1.749529265654429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.8615440086535034</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.8699571331276832</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-0.8699571331276833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.8795721325267457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-1.000000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>3.604823524698546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1.855294259044117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1.855294259044117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>1.855294259044118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>2.793037137935192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>-2.793037137935192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-2.761548014903262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2.761548014903262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1.705781018388694</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-0.03365249789671901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.006970874564320367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.4106806618324632</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.4003445374784709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>1.534313529105413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>-0.008893874444132883</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>-2.844116822242711</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-0.7966027002123338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>0.7966027002123338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>4.192500300468752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>1.060414246224113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>1.060414246224113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0.008893874444132883</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>2.881211122307894e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>5.688233644485422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-0.2072032370497985</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>0.2072032370497985</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.005047874684507852</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0.005047874684507852</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0.1139377428788915</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-0.02067224870798434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0.02067224870798434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0.02403749849765644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0.02403749849765644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0.006970874564320367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>0.4106806618324632</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2466,7 +2466,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>1.032290372981856</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2490,7 +2490,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>1.032290372981856</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>2.742558391090113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>3.709466768158342</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>-0.8653499459156319</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>-1.032290372981856</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2690,7 +2690,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>1.799447137534562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>-1.101037618685153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>-0.7671567645527064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>1.000000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>-2.611073274307932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>-2.611073274307932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2930,7 +2930,7 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>-2.611073274307932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>-2.611073274307932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:2">

</xml_diff>

<commit_message>
Revert "Removing remaining knock outs from iFerment"
This reverts commit 64be93cdc26ee6bdbec2398feebd28468a31ba4c.
</commit_message>
<xml_diff>
--- a/iFermentAsPacidpropionici.xlsx
+++ b/iFermentAsPacidpropionici.xlsx
@@ -1218,7 +1218,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-1.749529265654429</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.8615440086535034</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>-0.8699571331276832</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>-0.8699571331276833</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>-0.8795721325267457</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>-1.000000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>3.604823524698546</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1.855294259044117</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1.855294259044117</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1.855294259044118</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>2.793037137935192</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>-2.793037137935192</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-2.761548014903262</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>2.761548014903262</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1.705781018388694</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-0.03365249789671901</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>0.006970874564320367</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.4106806618324632</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.4003445374784709</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1.534313529105413</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>-0.008893874444132883</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>-2.844116822242711</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>-0.7966027002123338</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>0.7966027002123338</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>4.192500300468752</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>1.060414246224113</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>1.060414246224113</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>0.008893874444132883</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>2.881211122307894e-16</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>5.688233644485422</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>0</v>
+        <v>-0.2072032370497985</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>0.2072032370497985</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>-0.005047874684507852</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0</v>
+        <v>0.005047874684507852</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>0.1139377428788915</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>0</v>
+        <v>-0.02067224870798434</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>0.02067224870798434</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>0.02403749849765644</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0</v>
+        <v>0.02403749849765644</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>0.006970874564320367</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>0</v>
+        <v>0.4106806618324632</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2466,7 +2466,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>1.032290372981856</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2490,7 +2490,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>0</v>
+        <v>1.032290372981856</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>0</v>
+        <v>2.742558391090113</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>0</v>
+        <v>3.709466768158342</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>0</v>
+        <v>-0.8653499459156319</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>0</v>
+        <v>-1.032290372981856</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2690,7 +2690,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>0</v>
+        <v>1.799447137534562</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>0</v>
+        <v>-1.101037618685153</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>-0.7671567645527064</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>1.000000000000005</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>0</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>0</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2930,7 +2930,7 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>0</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>0</v>
+        <v>-2.611073274307932</v>
       </c>
     </row>
     <row r="230" spans="1:2">

</xml_diff>